<commit_message>
Learning continue and update the code
</commit_message>
<xml_diff>
--- a/Optimization/Lag/res.xlsx
+++ b/Optimization/Lag/res.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -388,7 +388,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.513677811550152</v>
+        <v>6.231578947368421</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -402,13 +402,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>17.16</v>
+        <v>0.7523364485981308</v>
       </c>
       <c r="C3">
-        <v>3.090908894620767</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3.09090909090909</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -416,13 +416,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.307692307692308</v>
+        <v>6.176887871853547</v>
       </c>
       <c r="C4">
-        <v>9.357141295478602</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>9.357142857142858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -430,7 +430,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.589743589743589</v>
+        <v>1.194444444444445</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -444,7 +444,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>13.99720540288775</v>
+        <v>1.886792452830189</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>7.157142857142857</v>
+        <v>4.882959979864082</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -472,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5.526315789473685</v>
+        <v>2.167660702451955</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -486,13 +486,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.9090909090909083</v>
+        <v>2.489878542510121</v>
       </c>
       <c r="C9">
-        <v>3.649998912319944</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>3.649999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -500,7 +500,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>7.02701115678215</v>
+        <v>2.946332737030411</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -514,13 +514,1273 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5454545454545463</v>
+        <v>3.463157894736842</v>
       </c>
       <c r="C11">
-        <v>1.952376918874783</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1.952380952380949</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>5.700348432055749</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2.656514382402707</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2.674228103339635</v>
+      </c>
+      <c r="C14">
+        <v>0.003173204492782133</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.6298003072196617</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2.272596843615495</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.2438618393674576</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1.898705255140899</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1.886257309941519</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1.925925925925926</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>1.044303797468355</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>4.869565217391305</v>
+      </c>
+      <c r="C22">
+        <v>0.007926499272713272</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0.5059523809523814</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>2.051282051282051</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.2433734939759042</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>3.346666666666668</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>2.026315789473684</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>2.877049180327869</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>4.960975609756098</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>3.617224880382775</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>4.536786469344609</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>7.245249926921955</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>4.115145228215767</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>3.860294117647059</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0.6572580645161289</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.6187581415544905</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>3.442975206611571</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0.2215208034433283</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>4.840579710144928</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0.6617647058823524</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>3.107480029048657</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>2.961038961038961</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>0.4571841155234648</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>1.918055555555555</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>1.051282051282049</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>2.644599303135888</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>0.9550561797752755</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>4.013452914798206</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>0.6146926536731625</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>1.873469387755101</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>4.440892098500626e-16</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>7.794979079497907</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>1.766801619433199</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>3.954859511745738</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>3.743462343096236</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>3.542202478372691</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>1.090909090909092</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>5.738823529411764</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>11.25595238095238</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>0.6542646542646542</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>0.5910931174089069</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>5.134814814814815</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>0.3684210526315798</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>2.407894736842105</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>0.9148760330578503</v>
+      </c>
+      <c r="C66">
+        <v>7.105427357601002e-15</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>6.384863123993559</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>0.4761904761904763</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>3.139130434782605</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>2.38877551020408</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>0.552517985611511</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>1.754310344827586</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>4.312903225806451</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>8.797058823529412</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>4.172557172557173</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>1.327058823529412</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>3.584</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>6.3710407239819</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>1.870689655172413</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>0.06617647058823595</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>2.19556451612903</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>0.3034410844629822</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>4.477064220183487</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>0.8933739527798936</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>5.212765957446807</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>0.1666666666666665</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>0.6892086330935251</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>3.147058823529412</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>5.086956521739133</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>3.94871794871795</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>5.283597725231967</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>4.650446871896726</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>0.3462397617274764</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>4.932502596053998</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>0.6300897170462403</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>1.805194805194809</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>0.338680926916223</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>3.036979969183359</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>